<commit_message>
finish the grouping code
</commit_message>
<xml_diff>
--- a/outputs/output.xlsx
+++ b/outputs/output.xlsx
@@ -569,40 +569,40 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.00702351814408854</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>0.00585293178674045</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>0.00702351814408854</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>421</v>
+        <v>867</v>
       </c>
       <c r="J4" s="4" t="n">
-        <v>0.0448015324039587</v>
+        <v>0.10610696365194</v>
       </c>
       <c r="K4" t="n">
-        <v>6084</v>
+        <v>6679</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>0.647440672555071</v>
+        <v>0.817403010647412</v>
       </c>
       <c r="M4" t="n">
-        <v>606</v>
+        <v>472</v>
       </c>
       <c r="N4" s="4" t="n">
-        <v>0.064488666595722</v>
+        <v>0.0577652674091299</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -611,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>2099</v>
+        <v>153</v>
       </c>
       <c r="R4" s="4" t="n">
-        <v>0.223369160370331</v>
+        <v>0.0187247582915188</v>
       </c>
       <c r="S4" t="n">
-        <v>9397</v>
+        <v>8171</v>
       </c>
       <c r="T4" s="4" t="n">
         <v>1</v>
@@ -628,81 +628,180 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.00927542557835007</v>
+        <v>0.0145332050048123</v>
       </c>
       <c r="E5" t="n">
-        <v>490</v>
+        <v>545</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>0.0534701003928416</v>
+        <v>0.0524542829643888</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>0</v>
+        <v>0.00635226179018287</v>
       </c>
       <c r="I5" t="n">
-        <v>446</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>0.0486687036228721</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>644</v>
+        <v>49</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>0.0702749890877346</v>
+        <v>0.00471607314725698</v>
       </c>
       <c r="M5" t="n">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>0.00120034919249236</v>
+        <v>0.0139557266602502</v>
       </c>
       <c r="O5" t="n">
         <v>280</v>
       </c>
       <c r="P5" s="4" t="n">
-        <v>0.0305543430816237</v>
+        <v>0.026948989412897</v>
       </c>
       <c r="Q5" t="n">
-        <v>7208</v>
+        <v>9154</v>
       </c>
       <c r="R5" s="4" t="n">
-        <v>0.786556089044086</v>
+        <v>0.881039461020212</v>
       </c>
       <c r="S5" t="n">
-        <v>9164</v>
+        <v>10390</v>
       </c>
       <c r="T5" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="D6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="T6" s="4"/>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>66</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0.00702351814408854</v>
+      </c>
+      <c r="E6" t="n">
+        <v>55</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0.00585293178674045</v>
+      </c>
+      <c r="G6" t="n">
+        <v>66</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>0.00702351814408854</v>
+      </c>
+      <c r="I6" t="n">
+        <v>421</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>0.0448015324039587</v>
+      </c>
+      <c r="K6" t="n">
+        <v>6084</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>0.647440672555071</v>
+      </c>
+      <c r="M6" t="n">
+        <v>606</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <v>0.064488666595722</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2099</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <v>0.223369160370331</v>
+      </c>
+      <c r="S6" t="n">
+        <v>9397</v>
+      </c>
+      <c r="T6" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
-      <c r="D7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="n">
+        <v>85</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0.00927542557835007</v>
+      </c>
+      <c r="E7" t="n">
+        <v>490</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0.0534701003928416</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>446</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>0.0486687036228721</v>
+      </c>
+      <c r="K7" t="n">
+        <v>644</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>0.0702749890877346</v>
+      </c>
+      <c r="M7" t="n">
+        <v>11</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>0.00120034919249236</v>
+      </c>
+      <c r="O7" t="n">
+        <v>280</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>0.0305543430816237</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7208</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>0.786556089044086</v>
+      </c>
+      <c r="S7" t="n">
+        <v>9164</v>
+      </c>
+      <c r="T7" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="D8" s="4"/>
@@ -736,19 +835,6 @@
       <c r="P10" s="4"/>
       <c r="R10" s="4"/>
       <c r="T10" s="4"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>